<commit_message>
add environment requirements to docs
</commit_message>
<xml_diff>
--- a/docs/MentorshipPlan.xlsx
+++ b/docs/MentorshipPlan.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Docs" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan" sheetId="2" r:id="rId1"/>
+    <sheet name="Docs" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Single responsibility principle</t>
   </si>
@@ -44,6 +45,48 @@
   </si>
   <si>
     <t>Parallel test runs -&gt; Data driven testing</t>
+  </si>
+  <si>
+    <t>Application:</t>
+  </si>
+  <si>
+    <t>https://www.rememberthemilk.com/</t>
+  </si>
+  <si>
+    <t>Setup environment:</t>
+  </si>
+  <si>
+    <t>IDE (Eclipse/IDEA)</t>
+  </si>
+  <si>
+    <t>Maven</t>
+  </si>
+  <si>
+    <t>TestNG</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Selenium WebDriver</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Firebug addons for Firefox</t>
+  </si>
+  <si>
+    <t>FirePath addons for Firefox</t>
+  </si>
+  <si>
+    <t>Firefox browser</t>
+  </si>
+  <si>
+    <t>Beyond Compare</t>
   </si>
 </sst>
 </file>
@@ -396,10 +439,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>